<commit_message>
Adding cucumber framework set up for Generic and Specifics multiple ticket creation
</commit_message>
<xml_diff>
--- a/src/main/resources/data/excelData.xlsx
+++ b/src/main/resources/data/excelData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SeleniumSnowUpdatedScript\src\main\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miteshkumar\IdeaProjects\SNow_MultipleTicketsCreation\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7814EF4-017F-4CA8-BDFB-00BA9962755B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009F9C95-528B-4821-9A5E-C8870E9C9D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4428" yWindow="2136" windowWidth="17280" windowHeight="8880" xr2:uid="{B5083333-8607-4968-ADC4-059C13A90821}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B5083333-8607-4968-ADC4-059C13A90821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>execute</t>
   </si>
@@ -48,6 +49,18 @@
   </si>
   <si>
     <t>Access to Network</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Back Up WAN Circuit Down</t>
+  </si>
+  <si>
+    <t>Broken keyboard or Mouse</t>
+  </si>
+  <si>
+    <t>Email Password Reset</t>
   </si>
 </sst>
 </file>
@@ -419,19 +432,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032EB01E-876C-4AF5-BC76-42CB9AE83FFC}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -439,12 +452,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C59EC7-C8D7-4D65-9EB4-50A77AB6D6E4}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>